<commit_message>
Further work on the report
</commit_message>
<xml_diff>
--- a/Solo2/docs/DummyEncoding.xlsx
+++ b/Solo2/docs/DummyEncoding.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="19520" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>Brand</t>
   </si>
@@ -57,16 +58,159 @@
   </si>
   <si>
     <t>Gaggle</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>p25</t>
+  </si>
+  <si>
+    <t>p50</t>
+  </si>
+  <si>
+    <t>p75</t>
+  </si>
+  <si>
+    <t>p100</t>
+  </si>
+  <si>
+    <t>brand1</t>
+  </si>
+  <si>
+    <t>brand2</t>
+  </si>
+  <si>
+    <t>brand3</t>
+  </si>
+  <si>
+    <t>price1</t>
+  </si>
+  <si>
+    <t>price2</t>
+  </si>
+  <si>
+    <t>processor1</t>
+  </si>
+  <si>
+    <t>processor2</t>
+  </si>
+  <si>
+    <t>RAM1</t>
+  </si>
+  <si>
+    <t>RAM2</t>
+  </si>
+  <si>
+    <t>screen1</t>
+  </si>
+  <si>
+    <t>screen2</t>
+  </si>
+  <si>
+    <t>brand0</t>
+  </si>
+  <si>
+    <t>price0</t>
+  </si>
+  <si>
+    <t>processor0</t>
+  </si>
+  <si>
+    <t>RAM0</t>
+  </si>
+  <si>
+    <t>screen0</t>
+  </si>
+  <si>
+    <t>1.5g</t>
+  </si>
+  <si>
+    <t>2g</t>
+  </si>
+  <si>
+    <t>2.5g</t>
+  </si>
+  <si>
+    <t>8gb</t>
+  </si>
+  <si>
+    <t>16gb</t>
+  </si>
+  <si>
+    <t>32gb</t>
+  </si>
+  <si>
+    <t>5inch</t>
+  </si>
+  <si>
+    <t>7inch</t>
+  </si>
+  <si>
+    <t>10inch</t>
+  </si>
+  <si>
+    <t>pref over baseline</t>
+  </si>
+  <si>
+    <t>odds-ratio(mean)</t>
+  </si>
+  <si>
+    <t>preference over mean baseline</t>
+  </si>
+  <si>
+    <t>1.5Ghz</t>
+  </si>
+  <si>
+    <t>2Ghz</t>
+  </si>
+  <si>
+    <t>2.5Ghz</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,13 +233,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -373,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,4 +628,899 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <f>-SUM(C3:C5)</f>
+        <v>0.432</v>
+      </c>
+      <c r="D2" s="7">
+        <f>EXP(C2)</f>
+        <v>1.5403351151611271</v>
+      </c>
+      <c r="H2" s="2">
+        <f>-SUM(H3:H5)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>-0.22</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D17" si="0">EXP(C3)</f>
+        <v>0.80251879796247849</v>
+      </c>
+      <c r="E3">
+        <v>0.86</v>
+      </c>
+      <c r="F3">
+        <v>-4.28</v>
+      </c>
+      <c r="G3">
+        <v>-0.33</v>
+      </c>
+      <c r="H3" s="3">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.13</v>
+      </c>
+      <c r="J3">
+        <v>2.77</v>
+      </c>
+      <c r="K3" s="4">
+        <f>EXP(H3-$H$2)</f>
+        <v>0.90032452258626561</v>
+      </c>
+      <c r="L3" s="4">
+        <f>EXP(C3-$C$2)</f>
+        <v>0.52100272860333441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0919881220281975</v>
+      </c>
+      <c r="E4">
+        <v>1.6</v>
+      </c>
+      <c r="F4">
+        <v>-5.85</v>
+      </c>
+      <c r="G4">
+        <v>-0.26</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="I4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J4">
+        <v>6.65</v>
+      </c>
+      <c r="K4" s="4">
+        <f>EXP(H4-$H$2)</f>
+        <v>1.1297541017803188</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" ref="L4:L5" si="1">EXP(C4-$C$2)</f>
+        <v>0.7089289280495108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>-0.3</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.74081822068171788</v>
+      </c>
+      <c r="E5">
+        <v>1.4</v>
+      </c>
+      <c r="F5">
+        <v>-5.24</v>
+      </c>
+      <c r="G5">
+        <v>-0.46</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-4.1000000000000002E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.3</v>
+      </c>
+      <c r="J5">
+        <v>5.96</v>
+      </c>
+      <c r="K5" s="4">
+        <f>EXP(H5-$H$2)</f>
+        <v>0.95218112969850488</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48094613528577801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5">
+        <v>199</v>
+      </c>
+      <c r="C6" s="2">
+        <f>-SUM(C7:C8)</f>
+        <v>2.61</v>
+      </c>
+      <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>13.599050851830924</v>
+      </c>
+      <c r="H6" s="2">
+        <f>-SUM(H7:H8)</f>
+        <v>1.7799999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6">
+        <v>299</v>
+      </c>
+      <c r="C7">
+        <v>0.31</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>1.3634251141321778</v>
+      </c>
+      <c r="E7">
+        <v>0.35</v>
+      </c>
+      <c r="F7">
+        <v>-0.74</v>
+      </c>
+      <c r="G7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="I7">
+        <v>0.52</v>
+      </c>
+      <c r="J7">
+        <v>1.55</v>
+      </c>
+      <c r="K7" s="4">
+        <f>EXP(H7-$H$6)</f>
+        <v>0.2299254851867239</v>
+      </c>
+      <c r="L7" s="4">
+        <f>EXP(C7-$C$6)</f>
+        <v>0.10025884372280375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6">
+        <v>399</v>
+      </c>
+      <c r="C8">
+        <v>-2.92</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3933687300356019E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.83</v>
+      </c>
+      <c r="F8">
+        <v>-9.76</v>
+      </c>
+      <c r="G8">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="H8" s="3">
+        <v>-2.09</v>
+      </c>
+      <c r="I8">
+        <v>-0.61</v>
+      </c>
+      <c r="J8">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="K8" s="4">
+        <f>EXP(H8-$H$6)</f>
+        <v>2.0858369425214726E-2</v>
+      </c>
+      <c r="L8" s="4">
+        <f>EXP(C8-$C$6)</f>
+        <v>3.9659890890910683E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2">
+        <f>-SUM(C10:C11)</f>
+        <v>-2.35</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>9.5369162215549613E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <f>-SUM(H10:H11)</f>
+        <v>-1.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>1.03</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8010658346990791</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>-1.33</v>
+      </c>
+      <c r="G10">
+        <v>0.26</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="I10">
+        <v>1.74</v>
+      </c>
+      <c r="J10">
+        <v>3.54</v>
+      </c>
+      <c r="K10" s="4">
+        <f>EXP(H10-$H$9)</f>
+        <v>14.439969192802881</v>
+      </c>
+      <c r="L10" s="4">
+        <f>EXP(C10-$C$9)</f>
+        <v>29.370771113289432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11">
+        <v>1.32</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7434213772608627</v>
+      </c>
+      <c r="E11">
+        <v>1.08</v>
+      </c>
+      <c r="F11">
+        <v>-1.5</v>
+      </c>
+      <c r="G11">
+        <v>0.38</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="I11">
+        <v>2.12</v>
+      </c>
+      <c r="J11">
+        <v>3.8</v>
+      </c>
+      <c r="K11" s="4">
+        <f>EXP(H11-$H$9)</f>
+        <v>18.915846312255049</v>
+      </c>
+      <c r="L11" s="4">
+        <f>EXP(C11-$C$9)</f>
+        <v>39.251905860304497</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2">
+        <f>-SUM(C13:C14)</f>
+        <v>-0.72499999999999998</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>0.48432456895536247</v>
+      </c>
+      <c r="H12" s="2">
+        <f>-SUM(H13:H14)</f>
+        <v>-0.6429999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0887170666983987</v>
+      </c>
+      <c r="E13">
+        <v>0.24</v>
+      </c>
+      <c r="F13">
+        <v>-0.46</v>
+      </c>
+      <c r="G13">
+        <v>-7.8E-2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.23</v>
+      </c>
+      <c r="J13">
+        <v>1.04</v>
+      </c>
+      <c r="K13" s="4">
+        <f>EXP(H13-$H$12)</f>
+        <v>2.0462318913749393</v>
+      </c>
+      <c r="L13" s="4">
+        <f>EXP(C13-$C$12)</f>
+        <v>2.2479079866764713</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>0.64</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8964808793049515</v>
+      </c>
+      <c r="E14">
+        <v>0.6</v>
+      </c>
+      <c r="F14">
+        <v>-0.77</v>
+      </c>
+      <c r="G14">
+        <v>0.17</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I14">
+        <v>1.03</v>
+      </c>
+      <c r="J14">
+        <v>2.42</v>
+      </c>
+      <c r="K14" s="4">
+        <f>EXP(H14-$H$12)</f>
+        <v>3.3635602122896127</v>
+      </c>
+      <c r="L14" s="4">
+        <f>EXP(C14-$C$12)</f>
+        <v>3.915723051992722</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2">
+        <f>-SUM(C16:C17)</f>
+        <v>-0.26999999999999996</v>
+      </c>
+      <c r="D15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.76337949433685326</v>
+      </c>
+      <c r="H15" s="2">
+        <f>-SUM(H16:H17)</f>
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>-0.2</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.81873075307798182</v>
+      </c>
+      <c r="E16">
+        <v>0.59</v>
+      </c>
+      <c r="F16">
+        <v>-2.83</v>
+      </c>
+      <c r="G16">
+        <v>-0.42</v>
+      </c>
+      <c r="H16" s="3">
+        <v>-0.12</v>
+      </c>
+      <c r="I16">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J16">
+        <v>1.53</v>
+      </c>
+      <c r="K16" s="4">
+        <f>EXP(H16-$H$15)</f>
+        <v>1.1853048513203654</v>
+      </c>
+      <c r="L16" s="4">
+        <f>EXP(C16-$C$15)</f>
+        <v>1.0725081812542163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>0.47</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5999941932173602</v>
+      </c>
+      <c r="E17">
+        <v>0.62</v>
+      </c>
+      <c r="F17">
+        <v>-0.84</v>
+      </c>
+      <c r="G17">
+        <v>-3.2000000000000003E-4</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="I17">
+        <v>0.9</v>
+      </c>
+      <c r="J17">
+        <v>2.74</v>
+      </c>
+      <c r="K17" s="4">
+        <f>EXP(H17-$H$15)</f>
+        <v>2.0137527074704766</v>
+      </c>
+      <c r="L17" s="4">
+        <f>EXP(C17-$C$15)</f>
+        <v>2.0959355144943643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.432</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.5403351151611271</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="4">
+        <v>-0.22</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.80251879796247849</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.52100272860333441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1.0919881220281975</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.7089289280495108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4">
+        <v>-0.3</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.74081822068171788</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.48094613528577801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="8">
+        <v>199</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2.61</v>
+      </c>
+      <c r="D25" s="4">
+        <v>13.599050851830924</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="8">
+        <v>299</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.31</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1.3634251141321778</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.10025884372280375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="8">
+        <v>399</v>
+      </c>
+      <c r="C27" s="4">
+        <v>-2.92</v>
+      </c>
+      <c r="D27" s="4">
+        <v>5.3933687300356019E-2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>3.9659890890910683E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="4">
+        <v>-2.35</v>
+      </c>
+      <c r="D28" s="4">
+        <v>9.5369162215549613E-2</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="D29" s="4">
+        <v>2.8010658346990791</v>
+      </c>
+      <c r="E29" s="4">
+        <v>29.370771113289432</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1.32</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3.7434213772608627</v>
+      </c>
+      <c r="E30" s="4">
+        <v>39.251905860304497</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="4">
+        <v>-0.72499999999999998</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.48432456895536247</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.0887170666983987</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.2479079866764713</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.64</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.8964808793049515</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3.915723051992722</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="4">
+        <v>-0.26999999999999996</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.76337949433685326</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="4">
+        <v>-0.2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.81873075307798182</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1.0725081812542163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.47</v>
+      </c>
+      <c r="D36" s="4">
+        <v>1.5999941932173602</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.0959355144943643</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>